<commit_message>
Exporting odds to excel file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="169">
   <si>
     <t>Sport Group</t>
   </si>
@@ -119,169 +119,169 @@
     <t>CCT European Series</t>
   </si>
   <si>
+    <t>RUBY</t>
+  </si>
+  <si>
+    <t>JANO Esports</t>
+  </si>
+  <si>
+    <t>Team Sampi</t>
+  </si>
+  <si>
+    <t>NOM</t>
+  </si>
+  <si>
+    <t>Illuminar Gaming</t>
+  </si>
+  <si>
+    <t>Elisa Invitational</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>Zero Tenacity</t>
+  </si>
+  <si>
+    <t>HAVU Gaming</t>
+  </si>
+  <si>
+    <t>ALTERNATE aTTaX</t>
+  </si>
+  <si>
+    <t>ESL Challenger League EU</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Apeks</t>
+  </si>
+  <si>
+    <t>Sprout</t>
+  </si>
+  <si>
+    <t>System 5</t>
+  </si>
+  <si>
+    <t>9INE</t>
+  </si>
+  <si>
+    <t>ESL Impact League EU</t>
+  </si>
+  <si>
+    <t>BIG EQUIPA</t>
+  </si>
+  <si>
+    <t>NIP Impact</t>
+  </si>
+  <si>
+    <t>ENCE Athena</t>
+  </si>
+  <si>
+    <t>Astralis Women</t>
+  </si>
+  <si>
+    <t>1win Gang</t>
+  </si>
+  <si>
+    <t>Fearless Cheetahs</t>
+  </si>
+  <si>
+    <t>Team Pigeons</t>
+  </si>
+  <si>
+    <t>Guild Esports</t>
+  </si>
+  <si>
+    <t>NAVI Javelins</t>
+  </si>
+  <si>
+    <t>VP.Angels</t>
+  </si>
+  <si>
+    <t>ESL Impact League NA</t>
+  </si>
+  <si>
+    <t>WG Bandits</t>
+  </si>
+  <si>
+    <t>COVEN</t>
+  </si>
+  <si>
+    <t>Team Karma</t>
+  </si>
+  <si>
+    <t>cleanup crew</t>
+  </si>
+  <si>
+    <t>Limitless Angels</t>
+  </si>
+  <si>
+    <t>Shimmer</t>
+  </si>
+  <si>
+    <t>ESL Impact League SA</t>
+  </si>
+  <si>
+    <t>Fluxo Demons</t>
+  </si>
+  <si>
+    <t>FURIA Esports Female</t>
+  </si>
+  <si>
+    <t>GENKID4M4</t>
+  </si>
+  <si>
+    <t>MIBR Female</t>
+  </si>
+  <si>
+    <t>KG Network Female</t>
+  </si>
+  <si>
+    <t>Atrix Esports</t>
+  </si>
+  <si>
+    <t>European Pro League</t>
+  </si>
+  <si>
+    <t>mouz NXT</t>
+  </si>
+  <si>
+    <t>Alliance</t>
+  </si>
+  <si>
+    <t>Dynamo Eclot</t>
+  </si>
+  <si>
+    <t>Global Esports Tour</t>
+  </si>
+  <si>
+    <t>Imperial Esports</t>
+  </si>
+  <si>
+    <t>Metizport</t>
+  </si>
+  <si>
+    <t>FURIA Esports</t>
+  </si>
+  <si>
+    <t>9z</t>
+  </si>
+  <si>
+    <t>MIBR</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>RES European Series</t>
+  </si>
+  <si>
+    <t>9 Pandas</t>
+  </si>
+  <si>
     <t>Sangal</t>
-  </si>
-  <si>
-    <t>Zero Tenacity</t>
-  </si>
-  <si>
-    <t>RUBY</t>
-  </si>
-  <si>
-    <t>JANO Esports</t>
-  </si>
-  <si>
-    <t>Team Sampi</t>
-  </si>
-  <si>
-    <t>NOM</t>
-  </si>
-  <si>
-    <t>Illuminar Gaming</t>
-  </si>
-  <si>
-    <t>Elisa Invitational</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>HAVU Gaming</t>
-  </si>
-  <si>
-    <t>ALTERNATE aTTaX</t>
-  </si>
-  <si>
-    <t>ESL Challenger League EU</t>
-  </si>
-  <si>
-    <t>Space</t>
-  </si>
-  <si>
-    <t>Apeks</t>
-  </si>
-  <si>
-    <t>Sprout</t>
-  </si>
-  <si>
-    <t>System 5</t>
-  </si>
-  <si>
-    <t>9INE</t>
-  </si>
-  <si>
-    <t>ESL Impact League EU</t>
-  </si>
-  <si>
-    <t>BIG EQUIPA</t>
-  </si>
-  <si>
-    <t>NIP Impact</t>
-  </si>
-  <si>
-    <t>ENCE Athena</t>
-  </si>
-  <si>
-    <t>Astralis Women</t>
-  </si>
-  <si>
-    <t>1win Gang</t>
-  </si>
-  <si>
-    <t>Fearless Cheetahs</t>
-  </si>
-  <si>
-    <t>Team Pigeons</t>
-  </si>
-  <si>
-    <t>Guild Esports</t>
-  </si>
-  <si>
-    <t>NAVI Javelins</t>
-  </si>
-  <si>
-    <t>VP.Angels</t>
-  </si>
-  <si>
-    <t>ESL Impact League NA</t>
-  </si>
-  <si>
-    <t>WG Bandits</t>
-  </si>
-  <si>
-    <t>COVEN</t>
-  </si>
-  <si>
-    <t>Team Karma</t>
-  </si>
-  <si>
-    <t>cleanup crew</t>
-  </si>
-  <si>
-    <t>Limitless Angels</t>
-  </si>
-  <si>
-    <t>Shimmer</t>
-  </si>
-  <si>
-    <t>ESL Impact League SA</t>
-  </si>
-  <si>
-    <t>Fluxo Demons</t>
-  </si>
-  <si>
-    <t>FURIA Esports Female</t>
-  </si>
-  <si>
-    <t>GENKID4M4</t>
-  </si>
-  <si>
-    <t>MIBR Female</t>
-  </si>
-  <si>
-    <t>KG Network Female</t>
-  </si>
-  <si>
-    <t>Atrix Esports</t>
-  </si>
-  <si>
-    <t>European Pro League</t>
-  </si>
-  <si>
-    <t>mouz NXT</t>
-  </si>
-  <si>
-    <t>Alliance</t>
-  </si>
-  <si>
-    <t>Dynamo Eclot</t>
-  </si>
-  <si>
-    <t>Global Esports Tour</t>
-  </si>
-  <si>
-    <t>Imperial Esports</t>
-  </si>
-  <si>
-    <t>Metizport</t>
-  </si>
-  <si>
-    <t>FURIA Esports</t>
-  </si>
-  <si>
-    <t>9z</t>
-  </si>
-  <si>
-    <t>MIBR</t>
-  </si>
-  <si>
-    <t>OG</t>
-  </si>
-  <si>
-    <t>RES European Series</t>
-  </si>
-  <si>
-    <t>9 Pandas</t>
   </si>
   <si>
     <t>PARIVISION</t>
@@ -563,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -783,10 +783,10 @@
         <v>23</v>
       </c>
       <c r="E11" t="n">
-        <v>1.55</v>
+        <v>2.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2.35</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="12">
@@ -903,10 +903,10 @@
         <v>36</v>
       </c>
       <c r="E17" t="n">
-        <v>1.16</v>
+        <v>1.29</v>
       </c>
       <c r="F17" t="n">
-        <v>4.7</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="18">
@@ -923,10 +923,10 @@
         <v>38</v>
       </c>
       <c r="E18" t="n">
-        <v>1.29</v>
+        <v>1.32</v>
       </c>
       <c r="F18" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="19">
@@ -937,16 +937,16 @@
         <v>34</v>
       </c>
       <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
       <c r="E19" t="n">
-        <v>1.32</v>
+        <v>1.63</v>
       </c>
       <c r="F19" t="n">
-        <v>3.2</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="20">
@@ -954,19 +954,19 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" t="n">
-        <v>1.63</v>
+        <v>1.46</v>
       </c>
       <c r="F20" t="n">
-        <v>2.23</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="21">
@@ -974,19 +974,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E21" t="n">
-        <v>1.46</v>
+        <v>3.85</v>
       </c>
       <c r="F21" t="n">
-        <v>2.63</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="22">
@@ -994,19 +994,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E22" t="n">
-        <v>3.85</v>
+        <v>1.65</v>
       </c>
       <c r="F22" t="n">
-        <v>1.23</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="23">
@@ -1014,19 +1014,19 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E23" t="n">
-        <v>1.65</v>
+        <v>1.2</v>
       </c>
       <c r="F23" t="n">
-        <v>2.2</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="24">
@@ -1034,19 +1034,19 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E24" t="n">
-        <v>1.2</v>
+        <v>1.52</v>
       </c>
       <c r="F24" t="n">
-        <v>4.2</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="25">
@@ -1054,19 +1054,19 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E25" t="n">
-        <v>1.52</v>
+        <v>1.48</v>
       </c>
       <c r="F25" t="n">
-        <v>2.48</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="26">
@@ -1074,19 +1074,19 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E26" t="n">
-        <v>1.48</v>
+        <v>1.38</v>
       </c>
       <c r="F26" t="n">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="27">
@@ -1094,19 +1094,19 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E27" t="n">
-        <v>1.38</v>
+        <v>7.0</v>
       </c>
       <c r="F27" t="n">
-        <v>2.9</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="28">
@@ -1114,19 +1114,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" t="n">
-        <v>7.0</v>
+        <v>1.3</v>
       </c>
       <c r="F28" t="n">
-        <v>1.08</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="29">
@@ -1134,19 +1134,19 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" t="n">
-        <v>1.3</v>
+        <v>1.02</v>
       </c>
       <c r="F29" t="n">
-        <v>3.35</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="30">
@@ -1154,19 +1154,19 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E30" t="n">
-        <v>1.02</v>
+        <v>1.23</v>
       </c>
       <c r="F30" t="n">
-        <v>12.5</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="31">
@@ -1174,19 +1174,19 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E31" t="n">
-        <v>1.23</v>
+        <v>1.25</v>
       </c>
       <c r="F31" t="n">
-        <v>3.85</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="32">
@@ -1194,19 +1194,19 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E32" t="n">
-        <v>1.25</v>
+        <v>3.25</v>
       </c>
       <c r="F32" t="n">
-        <v>3.65</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="33">
@@ -1214,19 +1214,19 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E33" t="n">
-        <v>3.25</v>
+        <v>2.33</v>
       </c>
       <c r="F33" t="n">
-        <v>1.32</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="34">
@@ -1234,19 +1234,19 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E34" t="n">
-        <v>2.33</v>
+        <v>7.5</v>
       </c>
       <c r="F34" t="n">
-        <v>1.57</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="35">
@@ -1254,19 +1254,19 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E35" t="n">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="F35" t="n">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="36">
@@ -1274,19 +1274,19 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="E36" t="n">
-        <v>8.5</v>
+        <v>1.11</v>
       </c>
       <c r="F36" t="n">
-        <v>1.06</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="37">
@@ -1294,19 +1294,19 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>78</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E37" t="n">
-        <v>1.11</v>
+        <v>2.08</v>
       </c>
       <c r="F37" t="n">
-        <v>5.8</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="38">
@@ -1314,19 +1314,19 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E38" t="n">
-        <v>2.08</v>
+        <v>1.36</v>
       </c>
       <c r="F38" t="n">
-        <v>1.71</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="39">
@@ -1334,19 +1334,19 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E39" t="n">
-        <v>1.36</v>
+        <v>1.54</v>
       </c>
       <c r="F39" t="n">
-        <v>3.0</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="40">
@@ -1354,19 +1354,19 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E40" t="n">
-        <v>1.54</v>
+        <v>1.86</v>
       </c>
       <c r="F40" t="n">
-        <v>2.43</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="41">
@@ -1374,19 +1374,19 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E41" t="n">
-        <v>1.86</v>
+        <v>1.19</v>
       </c>
       <c r="F41" t="n">
-        <v>1.9</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="42">
@@ -1394,19 +1394,19 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E42" t="n">
-        <v>1.19</v>
+        <v>1.58</v>
       </c>
       <c r="F42" t="n">
-        <v>4.3</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="43">
@@ -1414,19 +1414,19 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="E43" t="n">
-        <v>1.58</v>
+        <v>1.66</v>
       </c>
       <c r="F43" t="n">
-        <v>2.32</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="44">
@@ -1434,19 +1434,19 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E44" t="n">
-        <v>1.66</v>
+        <v>1.12</v>
       </c>
       <c r="F44" t="n">
-        <v>2.17</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="45">
@@ -1454,19 +1454,19 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="D45" t="s">
         <v>44</v>
       </c>
       <c r="E45" t="n">
-        <v>1.12</v>
+        <v>1.48</v>
       </c>
       <c r="F45" t="n">
-        <v>5.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="46">
@@ -1474,19 +1474,19 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E46" t="n">
-        <v>1.48</v>
+        <v>1.7</v>
       </c>
       <c r="F46" t="n">
-        <v>2.6</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="47">
@@ -1494,19 +1494,19 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="E47" t="n">
-        <v>1.7</v>
+        <v>1.64</v>
       </c>
       <c r="F47" t="n">
-        <v>2.12</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="48">
@@ -1514,19 +1514,19 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="E48" t="n">
-        <v>1.64</v>
+        <v>1.76</v>
       </c>
       <c r="F48" t="n">
-        <v>2.2</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="49">
@@ -1537,16 +1537,16 @@
         <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="E49" t="n">
-        <v>1.76</v>
+        <v>1.87</v>
       </c>
       <c r="F49" t="n">
-        <v>2.02</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="50">
@@ -1557,36 +1557,36 @@
         <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E50" t="n">
-        <v>1.87</v>
+        <v>1.77</v>
       </c>
       <c r="F50" t="n">
-        <v>1.9</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E51" t="n">
-        <v>1.77</v>
+        <v>1.44</v>
       </c>
       <c r="F51" t="n">
-        <v>2.0</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="52">
@@ -1594,19 +1594,19 @@
         <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E52" t="n">
-        <v>1.44</v>
+        <v>12.0</v>
       </c>
       <c r="F52" t="n">
-        <v>2.63</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="53">
@@ -1617,16 +1617,16 @@
         <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D53" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E53" t="n">
-        <v>3.4</v>
+        <v>6.25</v>
       </c>
       <c r="F53" t="n">
-        <v>1.28</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="54">
@@ -1637,16 +1637,16 @@
         <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E54" t="n">
-        <v>6.25</v>
+        <v>5.5</v>
       </c>
       <c r="F54" t="n">
-        <v>1.1</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="55">
@@ -1657,16 +1657,16 @@
         <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E55" t="n">
-        <v>4.7</v>
+        <v>1.57</v>
       </c>
       <c r="F55" t="n">
-        <v>1.16</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="56">
@@ -1674,39 +1674,39 @@
         <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D56" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E56" t="n">
-        <v>1.57</v>
+        <v>1.53</v>
       </c>
       <c r="F56" t="n">
-        <v>2.31</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E57" t="n">
-        <v>1.53</v>
+        <v>1.72</v>
       </c>
       <c r="F57" t="n">
-        <v>2.4</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="58">
@@ -1714,19 +1714,19 @@
         <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D58" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E58" t="n">
-        <v>1.42</v>
+        <v>1.13</v>
       </c>
       <c r="F58" t="n">
-        <v>2.7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="59">
@@ -1737,16 +1737,16 @@
         <v>116</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E59" t="n">
-        <v>1.13</v>
+        <v>1.56</v>
       </c>
       <c r="F59" t="n">
-        <v>5.2</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="60">
@@ -1757,16 +1757,16 @@
         <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E60" t="n">
-        <v>1.56</v>
+        <v>1.47</v>
       </c>
       <c r="F60" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="61">
@@ -1777,36 +1777,36 @@
         <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D61" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E61" t="n">
-        <v>1.47</v>
+        <v>1.9</v>
       </c>
       <c r="F61" t="n">
-        <v>2.5</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="C62" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D62" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E62" t="n">
-        <v>1.9</v>
+        <v>1.27</v>
       </c>
       <c r="F62" t="n">
-        <v>1.81</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="63">
@@ -1817,16 +1817,16 @@
         <v>126</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E63" t="n">
-        <v>1.27</v>
+        <v>6.0</v>
       </c>
       <c r="F63" t="n">
-        <v>3.4</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="64">
@@ -1837,16 +1837,16 @@
         <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E64" t="n">
-        <v>6.0</v>
+        <v>2.25</v>
       </c>
       <c r="F64" t="n">
-        <v>1.1</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="65">
@@ -1857,16 +1857,16 @@
         <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D65" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E65" t="n">
-        <v>2.25</v>
+        <v>1.17</v>
       </c>
       <c r="F65" t="n">
-        <v>1.57</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="66">
@@ -1880,13 +1880,13 @@
         <v>132</v>
       </c>
       <c r="D66" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E66" t="n">
-        <v>1.17</v>
+        <v>2.0</v>
       </c>
       <c r="F66" t="n">
-        <v>4.5</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="67">
@@ -1897,16 +1897,16 @@
         <v>126</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E67" t="n">
-        <v>2.0</v>
+        <v>1.4</v>
       </c>
       <c r="F67" t="n">
-        <v>1.72</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="68">
@@ -1914,19 +1914,19 @@
         <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C68" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D68" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E68" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F68" t="n">
-        <v>2.75</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="69">
@@ -1934,19 +1934,19 @@
         <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E69" t="n">
-        <v>1.3</v>
+        <v>2.65</v>
       </c>
       <c r="F69" t="n">
-        <v>3.3</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="70">
@@ -1957,16 +1957,16 @@
         <v>137</v>
       </c>
       <c r="C70" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D70" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E70" t="n">
-        <v>2.65</v>
+        <v>2.2</v>
       </c>
       <c r="F70" t="n">
-        <v>1.42</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="71">
@@ -1974,19 +1974,19 @@
         <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E71" t="n">
-        <v>2.2</v>
+        <v>1.23</v>
       </c>
       <c r="F71" t="n">
-        <v>1.6</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="72">
@@ -1994,19 +1994,19 @@
         <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="E72" t="n">
-        <v>1.23</v>
+        <v>5.5</v>
       </c>
       <c r="F72" t="n">
-        <v>3.75</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="73">
@@ -2017,16 +2017,16 @@
         <v>145</v>
       </c>
       <c r="C73" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="D73" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="E73" t="n">
-        <v>5.5</v>
+        <v>1.72</v>
       </c>
       <c r="F73" t="n">
-        <v>1.12</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="74">
@@ -2037,16 +2037,16 @@
         <v>145</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D74" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E74" t="n">
-        <v>1.72</v>
+        <v>3.5</v>
       </c>
       <c r="F74" t="n">
-        <v>2.04</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="75">
@@ -2057,16 +2057,16 @@
         <v>145</v>
       </c>
       <c r="C75" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D75" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E75" t="n">
-        <v>3.5</v>
+        <v>2.35</v>
       </c>
       <c r="F75" t="n">
-        <v>1.27</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="76">
@@ -2077,16 +2077,16 @@
         <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D76" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E76" t="n">
-        <v>2.35</v>
+        <v>1.45</v>
       </c>
       <c r="F76" t="n">
-        <v>1.54</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="77">
@@ -2097,16 +2097,16 @@
         <v>145</v>
       </c>
       <c r="C77" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="D77" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E77" t="n">
-        <v>1.45</v>
+        <v>1.07</v>
       </c>
       <c r="F77" t="n">
-        <v>2.65</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="78">
@@ -2114,19 +2114,19 @@
         <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E78" t="n">
-        <v>1.07</v>
+        <v>1.4</v>
       </c>
       <c r="F78" t="n">
-        <v>7.5</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="79">
@@ -2137,16 +2137,16 @@
         <v>155</v>
       </c>
       <c r="C79" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D79" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E79" t="n">
-        <v>1.4</v>
+        <v>3.65</v>
       </c>
       <c r="F79" t="n">
-        <v>2.75</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="80">
@@ -2157,16 +2157,16 @@
         <v>155</v>
       </c>
       <c r="C80" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D80" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E80" t="n">
-        <v>3.65</v>
+        <v>2.45</v>
       </c>
       <c r="F80" t="n">
-        <v>1.24</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="81">
@@ -2174,19 +2174,19 @@
         <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D81" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E81" t="n">
-        <v>2.45</v>
+        <v>1.65</v>
       </c>
       <c r="F81" t="n">
-        <v>1.49</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="82">
@@ -2197,16 +2197,16 @@
         <v>162</v>
       </c>
       <c r="C82" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D82" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E82" t="n">
-        <v>1.65</v>
+        <v>6.0</v>
       </c>
       <c r="F82" t="n">
-        <v>2.1</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="83">
@@ -2217,35 +2217,15 @@
         <v>162</v>
       </c>
       <c r="C83" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D83" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E83" t="n">
-        <v>6.0</v>
+        <v>1.14</v>
       </c>
       <c r="F83" t="n">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>125</v>
-      </c>
-      <c r="B84" t="s">
-        <v>162</v>
-      </c>
-      <c r="C84" t="s">
-        <v>167</v>
-      </c>
-      <c r="D84" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="F84" t="n">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>